<commit_message>
Week 08 Numpy 01
</commit_message>
<xml_diff>
--- a/Week 04 MongoDB 01/FireForce_Character_Database.xlsx
+++ b/Week 04 MongoDB 01/FireForce_Character_Database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Abdullah\Documents\TTA Assignments\GitHub Repositories\TTA Data Science\Week 04 MongoDB 01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E718A8F-83DB-4EBA-838A-B7EE35053DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5344D07C-AC60-424E-AEEE-F9A906DECEB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7320" yWindow="-60" windowWidth="21600" windowHeight="11295" xr2:uid="{5F43DA51-5D09-4835-A21A-7A1EF0E0A3EA}"/>
   </bookViews>
@@ -708,18 +708,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -866,7 +860,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -934,30 +928,42 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -976,21 +982,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1003,70 +1009,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1387,10 +1339,10 @@
   <dimension ref="A1:R109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="M11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="R30" sqref="R30"/>
+      <selection pane="bottomRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1361,7 @@
     <col min="12" max="12" width="31.28515625" style="8" customWidth="1"/>
     <col min="13" max="13" width="25.7109375" style="8" customWidth="1"/>
     <col min="14" max="14" width="15.7109375" style="8" customWidth="1"/>
-    <col min="15" max="15" width="28.140625" style="40" customWidth="1"/>
+    <col min="15" max="15" width="28.140625" style="32" customWidth="1"/>
     <col min="16" max="16" width="22.85546875" style="8" customWidth="1"/>
     <col min="17" max="17" width="32.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="28.42578125" style="2" customWidth="1"/>
@@ -1417,20 +1369,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="29"/>
       <c r="D1" s="18"/>
       <c r="E1" s="15"/>
       <c r="F1" s="1"/>
       <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="39"/>
+      <c r="B2" s="31"/>
       <c r="D2" s="18"/>
       <c r="J2" s="18"/>
     </row>
@@ -1512,687 +1464,687 @@
       <c r="Q4" s="14"/>
       <c r="R4" s="13"/>
     </row>
-    <row r="5" spans="1:18" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="48" t="s">
+    <row r="5" spans="1:18" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="E5" s="52"/>
-      <c r="F5" s="50" t="s">
+      <c r="E5" s="37"/>
+      <c r="F5" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G5" s="50">
+      <c r="G5" s="35">
         <v>31</v>
       </c>
-      <c r="H5" s="52" t="s">
+      <c r="H5" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="50">
+      <c r="I5" s="35">
         <v>189</v>
       </c>
-      <c r="J5" s="53">
+      <c r="J5" s="38">
         <v>108</v>
       </c>
-      <c r="K5" s="50" t="s">
+      <c r="K5" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52" t="s">
+      <c r="M5" s="37"/>
+      <c r="N5" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="O5" s="52" t="s">
+      <c r="O5" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52" t="s">
+      <c r="P5" s="37"/>
+      <c r="Q5" s="37" t="s">
         <v>141</v>
       </c>
-      <c r="R5" s="54"/>
-    </row>
-    <row r="6" spans="1:18" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49" t="s">
+      <c r="R5" s="39"/>
+    </row>
+    <row r="6" spans="1:18" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="50"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="50" t="s">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="50"/>
-      <c r="L6" s="52"/>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="54"/>
-    </row>
-    <row r="7" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="49" t="s">
+      <c r="G6" s="35"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="39"/>
+    </row>
+    <row r="7" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F7" s="50" t="s">
+      <c r="F7" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="50"/>
-      <c r="H7" s="52"/>
-      <c r="I7" s="50"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="50"/>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52" t="s">
+      <c r="G7" s="35"/>
+      <c r="H7" s="37"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="N7" s="52"/>
-      <c r="O7" s="52"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="54" t="s">
+      <c r="N7" s="37"/>
+      <c r="O7" s="37"/>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="39" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="8" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49" t="s">
+    <row r="8" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G8" s="50"/>
-      <c r="H8" s="52"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="52"/>
-      <c r="M8" s="52"/>
-      <c r="N8" s="52"/>
-      <c r="O8" s="52"/>
-      <c r="P8" s="52"/>
-      <c r="Q8" s="52" t="s">
+      <c r="G8" s="35"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="37"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="37"/>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="R8" s="54"/>
-    </row>
-    <row r="9" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="49" t="s">
+      <c r="R8" s="39"/>
+    </row>
+    <row r="9" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="50" t="s">
+      <c r="C9" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="50" t="s">
+      <c r="E9" s="37"/>
+      <c r="F9" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="52"/>
-      <c r="I9" s="50"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="50"/>
-      <c r="L9" s="52"/>
-      <c r="M9" s="52"/>
-      <c r="N9" s="52"/>
-      <c r="O9" s="52"/>
-      <c r="P9" s="52" t="s">
+      <c r="G9" s="35"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="35"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="35"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="Q9" s="52" t="s">
+      <c r="Q9" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="R9" s="54"/>
-    </row>
-    <row r="10" spans="1:18" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="49" t="s">
+      <c r="R9" s="39"/>
+    </row>
+    <row r="10" spans="1:18" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="50"/>
-      <c r="D10" s="53" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="50">
+      <c r="G10" s="35">
         <v>24</v>
       </c>
-      <c r="H10" s="52" t="s">
+      <c r="H10" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="I10" s="50">
+      <c r="I10" s="35">
         <v>169</v>
       </c>
-      <c r="J10" s="53">
+      <c r="J10" s="38">
         <v>54</v>
       </c>
-      <c r="K10" s="50" t="s">
+      <c r="K10" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L10" s="52"/>
-      <c r="M10" s="52"/>
-      <c r="N10" s="52" t="s">
+      <c r="L10" s="37"/>
+      <c r="M10" s="37"/>
+      <c r="N10" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="O10" s="52" t="s">
+      <c r="O10" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="P10" s="52" t="s">
+      <c r="P10" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="Q10" s="52" t="s">
+      <c r="Q10" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="R10" s="54"/>
-    </row>
-    <row r="11" spans="1:18" s="55" customFormat="1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A11" s="48"/>
-      <c r="B11" s="49" t="s">
+      <c r="R10" s="39"/>
+    </row>
+    <row r="11" spans="1:18" s="40" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51" t="s">
+      <c r="C11" s="35"/>
+      <c r="D11" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="E11" s="52" t="s">
+      <c r="E11" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="F11" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G11" s="50">
+      <c r="G11" s="35">
         <v>17</v>
       </c>
-      <c r="H11" s="52" t="s">
+      <c r="H11" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="I11" s="50">
+      <c r="I11" s="35">
         <v>174</v>
       </c>
-      <c r="J11" s="53">
+      <c r="J11" s="38">
         <v>64</v>
       </c>
-      <c r="K11" s="50" t="s">
+      <c r="K11" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="52"/>
-      <c r="M11" s="52" t="s">
+      <c r="L11" s="37"/>
+      <c r="M11" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="N11" s="52" t="s">
+      <c r="N11" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="O11" s="52" t="s">
+      <c r="O11" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="P11" s="52"/>
-      <c r="Q11" s="52" t="s">
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="R11" s="54" t="s">
+      <c r="R11" s="39" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="12" spans="1:18" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="49" t="s">
+    <row r="12" spans="1:18" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="50"/>
-      <c r="D12" s="53" t="s">
+      <c r="C12" s="35"/>
+      <c r="D12" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="E12" s="52" t="s">
+      <c r="E12" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="G12" s="50"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="50"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="50"/>
-      <c r="L12" s="52"/>
-      <c r="M12" s="52"/>
-      <c r="N12" s="52" t="s">
+      <c r="G12" s="35"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="37"/>
+      <c r="N12" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52" t="s">
+      <c r="O12" s="37"/>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="R12" s="54" t="s">
+      <c r="R12" s="39" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:18" s="55" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="49" t="s">
+    <row r="13" spans="1:18" s="40" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="53" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="50" t="s">
+      <c r="F13" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G13" s="50">
+      <c r="G13" s="35">
         <v>28</v>
       </c>
-      <c r="H13" s="52" t="s">
+      <c r="H13" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="I13" s="50">
+      <c r="I13" s="35">
         <v>182</v>
       </c>
-      <c r="J13" s="53">
+      <c r="J13" s="38">
         <v>80</v>
       </c>
-      <c r="K13" s="50" t="s">
+      <c r="K13" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L13" s="52"/>
-      <c r="M13" s="52" t="s">
+      <c r="L13" s="37"/>
+      <c r="M13" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="N13" s="52"/>
-      <c r="O13" s="52" t="s">
+      <c r="N13" s="37"/>
+      <c r="O13" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="54"/>
-    </row>
-    <row r="14" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="49" t="s">
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="39"/>
+    </row>
+    <row r="14" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="50" t="s">
+      <c r="C14" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="F14" s="50" t="s">
+      <c r="F14" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="56"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="54"/>
-    </row>
-    <row r="15" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="G14" s="35"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="39"/>
+    </row>
+    <row r="15" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="49" t="s">
+      <c r="B15" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="56"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="52" t="s">
+      <c r="C15" s="43"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="60"/>
-    </row>
-    <row r="16" spans="1:18" s="55" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="61" t="s">
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="45"/>
+    </row>
+    <row r="16" spans="1:18" s="40" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="50"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52" t="s">
+      <c r="C16" s="35"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G16" s="50">
+      <c r="G16" s="35">
         <v>22</v>
       </c>
-      <c r="H16" s="52" t="s">
+      <c r="H16" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="I16" s="50">
+      <c r="I16" s="35">
         <v>170</v>
       </c>
-      <c r="J16" s="51">
+      <c r="J16" s="36">
         <v>62</v>
       </c>
-      <c r="K16" s="50" t="s">
+      <c r="K16" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L16" s="52" t="s">
+      <c r="L16" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="M16" s="52" t="s">
+      <c r="M16" s="37" t="s">
         <v>196</v>
       </c>
-      <c r="N16" s="52" t="s">
+      <c r="N16" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="O16" s="62" t="s">
+      <c r="O16" s="47" t="s">
         <v>173</v>
       </c>
-      <c r="P16" s="52" t="s">
+      <c r="P16" s="37" t="s">
         <v>175</v>
       </c>
-      <c r="Q16" s="52" t="s">
+      <c r="Q16" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="R16" s="54" t="s">
+      <c r="R16" s="39" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="17" spans="1:18" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="49" t="s">
+    <row r="17" spans="1:18" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="63" t="s">
+      <c r="C17" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="E17" s="62"/>
-      <c r="F17" s="63" t="s">
+      <c r="E17" s="47"/>
+      <c r="F17" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="G17" s="63"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="63"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="63"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="62"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="62"/>
-      <c r="R17" s="64"/>
-    </row>
-    <row r="18" spans="1:18" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="48" t="s">
+      <c r="G17" s="48"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="47"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="47"/>
+      <c r="O17" s="41"/>
+      <c r="P17" s="47"/>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="49"/>
+    </row>
+    <row r="18" spans="1:18" s="40" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59" t="s">
+      <c r="C18" s="43"/>
+      <c r="D18" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="F18" s="50" t="s">
+      <c r="F18" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G18" s="58">
+      <c r="G18" s="43">
         <v>28</v>
       </c>
-      <c r="H18" s="56" t="s">
+      <c r="H18" s="41" t="s">
         <v>182</v>
       </c>
-      <c r="I18" s="58">
+      <c r="I18" s="43">
         <v>202</v>
       </c>
-      <c r="J18" s="59">
+      <c r="J18" s="44">
         <v>130</v>
       </c>
-      <c r="K18" s="58"/>
-      <c r="L18" s="56" t="s">
+      <c r="K18" s="43"/>
+      <c r="L18" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="52" t="s">
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56" t="s">
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41" t="s">
         <v>183</v>
       </c>
-      <c r="R18" s="60"/>
-    </row>
-    <row r="19" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="61" t="s">
+      <c r="R18" s="45"/>
+    </row>
+    <row r="19" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="51" t="s">
+      <c r="C19" s="35"/>
+      <c r="D19" s="36" t="s">
         <v>146</v>
       </c>
-      <c r="E19" s="52"/>
-      <c r="F19" s="50" t="s">
+      <c r="E19" s="37"/>
+      <c r="F19" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="50"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="50"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="62"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="52" t="s">
+      <c r="G19" s="35"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="47"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="R19" s="54"/>
-    </row>
-    <row r="20" spans="1:18" s="55" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="48" t="s">
+      <c r="R19" s="39"/>
+    </row>
+    <row r="20" spans="1:18" s="40" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="E20" s="66"/>
-      <c r="F20" s="53" t="s">
+      <c r="E20" s="51"/>
+      <c r="F20" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="63"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="63"/>
-      <c r="J20" s="53"/>
-      <c r="K20" s="63"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62" t="s">
+      <c r="G20" s="48"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47" t="s">
         <v>189</v>
       </c>
-      <c r="O20" s="56"/>
-      <c r="P20" s="62" t="s">
+      <c r="O20" s="41"/>
+      <c r="P20" s="47" t="s">
         <v>188</v>
       </c>
-      <c r="Q20" s="62" t="s">
+      <c r="Q20" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="R20" s="64" t="s">
+      <c r="R20" s="49" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="1:18" s="55" customFormat="1" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="65" t="s">
+    <row r="21" spans="1:18" s="40" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="C21" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="58"/>
-      <c r="E21" s="67" t="s">
+      <c r="D21" s="43"/>
+      <c r="E21" s="52" t="s">
         <v>149</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="F21" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="58"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="59"/>
-      <c r="K21" s="58"/>
-      <c r="L21" s="56" t="s">
+      <c r="G21" s="43"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="44"/>
+      <c r="K21" s="43"/>
+      <c r="L21" s="41" t="s">
         <v>192</v>
       </c>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="52"/>
-      <c r="P21" s="56" t="s">
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="37"/>
+      <c r="P21" s="41" t="s">
         <v>191</v>
       </c>
-      <c r="Q21" s="56" t="s">
+      <c r="Q21" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="R21" s="60"/>
-    </row>
-    <row r="22" spans="1:18" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="R21" s="45"/>
+    </row>
+    <row r="22" spans="1:18" s="40" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="42" t="s">
+      <c r="B22" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="32" t="s">
+      <c r="D22" s="35"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="36" t="s">
         <v>147</v>
       </c>
-      <c r="G22" s="31"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="43"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33" t="s">
+      <c r="G22" s="35"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="37"/>
+      <c r="M22" s="37"/>
+      <c r="N22" s="37"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="R22" s="35" t="s">
+      <c r="R22" s="39" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+    <row r="23" spans="1:18" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44" t="s">
+      <c r="C23" s="48"/>
+      <c r="D23" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="E23" s="46" t="s">
+      <c r="E23" s="51" t="s">
         <v>149</v>
       </c>
-      <c r="F23" s="34" t="s">
+      <c r="F23" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="G23" s="44"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="44"/>
-      <c r="L23" s="43"/>
-      <c r="M23" s="43" t="s">
+      <c r="G23" s="48"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="48"/>
+      <c r="L23" s="47"/>
+      <c r="M23" s="47" t="s">
         <v>197</v>
       </c>
-      <c r="N23" s="43"/>
+      <c r="N23" s="47"/>
       <c r="O23" s="41"/>
-      <c r="P23" s="43"/>
-      <c r="Q23" s="33" t="s">
+      <c r="P23" s="47"/>
+      <c r="Q23" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="R23" s="45"/>
+      <c r="R23" s="49"/>
     </row>
     <row r="24" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
@@ -2200,7 +2152,7 @@
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="28"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="18"/>
       <c r="G24" s="6"/>
       <c r="H24" s="16"/>
@@ -2213,7 +2165,7 @@
       <c r="O24" s="14"/>
       <c r="P24" s="16"/>
       <c r="Q24" s="16"/>
-      <c r="R24" s="24"/>
+      <c r="R24" s="23"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
@@ -2221,7 +2173,7 @@
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
-      <c r="E25" s="29"/>
+      <c r="E25" s="28"/>
       <c r="F25" s="22"/>
       <c r="G25" s="5"/>
       <c r="H25" s="14"/>
@@ -2245,7 +2197,7 @@
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="27"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="21"/>
       <c r="G26" s="7"/>
       <c r="H26" s="17"/>
@@ -2258,18 +2210,18 @@
       <c r="O26" s="8"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="17"/>
-      <c r="R26" s="25"/>
+      <c r="R26" s="24"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>39</v>
       </c>
       <c r="D27" s="2"/>
-      <c r="E27" s="28"/>
+      <c r="E27" s="27"/>
       <c r="F27" s="18"/>
       <c r="J27" s="18"/>
       <c r="O27" s="14"/>
-      <c r="R27" s="26"/>
+      <c r="R27" s="25"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="12" t="s">
@@ -2277,7 +2229,7 @@
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="29"/>
+      <c r="E28" s="28"/>
       <c r="F28" s="22"/>
       <c r="G28" s="5"/>
       <c r="H28" s="14"/>
@@ -2297,11 +2249,11 @@
         <v>41</v>
       </c>
       <c r="D29" s="2"/>
-      <c r="E29" s="28"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="18"/>
       <c r="J29" s="18"/>
       <c r="O29" s="14"/>
-      <c r="R29" s="26"/>
+      <c r="R29" s="25"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
@@ -2309,7 +2261,7 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="29"/>
+      <c r="E30" s="28"/>
       <c r="F30" s="22"/>
       <c r="G30" s="5"/>
       <c r="H30" s="14"/>
@@ -2333,7 +2285,7 @@
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="27"/>
+      <c r="E31" s="26"/>
       <c r="F31" s="21"/>
       <c r="G31" s="7"/>
       <c r="H31" s="17"/>
@@ -2346,7 +2298,7 @@
       <c r="O31" s="16"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="17"/>
-      <c r="R31" s="25"/>
+      <c r="R31" s="24"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
@@ -2354,7 +2306,7 @@
       </c>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="28"/>
+      <c r="E32" s="27"/>
       <c r="F32" s="18"/>
       <c r="G32" s="6"/>
       <c r="H32" s="16"/>
@@ -2367,7 +2319,7 @@
       <c r="O32" s="14"/>
       <c r="P32" s="16"/>
       <c r="Q32" s="16"/>
-      <c r="R32" s="24"/>
+      <c r="R32" s="23"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
@@ -2375,7 +2327,7 @@
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="29"/>
+      <c r="E33" s="28"/>
       <c r="F33" s="22"/>
       <c r="G33" s="5"/>
       <c r="H33" s="14"/>
@@ -2396,7 +2348,7 @@
       </c>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="27"/>
+      <c r="E34" s="26"/>
       <c r="F34" s="21"/>
       <c r="G34" s="7"/>
       <c r="H34" s="17"/>
@@ -2409,18 +2361,18 @@
       <c r="O34" s="8"/>
       <c r="P34" s="17"/>
       <c r="Q34" s="17"/>
-      <c r="R34" s="25"/>
+      <c r="R34" s="24"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="2"/>
-      <c r="E35" s="28"/>
+      <c r="E35" s="27"/>
       <c r="F35" s="18"/>
       <c r="J35" s="18"/>
       <c r="O35" s="14"/>
-      <c r="R35" s="26"/>
+      <c r="R35" s="25"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
@@ -2428,7 +2380,7 @@
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="29"/>
+      <c r="E36" s="28"/>
       <c r="F36" s="22"/>
       <c r="G36" s="5"/>
       <c r="H36" s="14"/>
@@ -2448,11 +2400,11 @@
         <v>50</v>
       </c>
       <c r="D37" s="2"/>
-      <c r="E37" s="28"/>
+      <c r="E37" s="27"/>
       <c r="F37" s="18"/>
       <c r="J37" s="18"/>
       <c r="O37" s="14"/>
-      <c r="R37" s="26"/>
+      <c r="R37" s="25"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
@@ -2460,7 +2412,7 @@
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="29"/>
+      <c r="E38" s="28"/>
       <c r="F38" s="22"/>
       <c r="G38" s="5"/>
       <c r="H38" s="14"/>
@@ -2484,7 +2436,7 @@
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="27"/>
+      <c r="E39" s="26"/>
       <c r="F39" s="21"/>
       <c r="G39" s="5"/>
       <c r="H39" s="14"/>
@@ -2504,11 +2456,11 @@
         <v>54</v>
       </c>
       <c r="D40" s="2"/>
-      <c r="E40" s="28"/>
+      <c r="E40" s="27"/>
       <c r="F40" s="18"/>
       <c r="J40" s="18"/>
       <c r="O40" s="14"/>
-      <c r="R40" s="26"/>
+      <c r="R40" s="25"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B41" s="12" t="s">
@@ -2516,7 +2468,7 @@
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
-      <c r="E41" s="29"/>
+      <c r="E41" s="28"/>
       <c r="F41" s="22"/>
       <c r="G41" s="5"/>
       <c r="H41" s="14"/>
@@ -2536,11 +2488,11 @@
         <v>56</v>
       </c>
       <c r="D42" s="2"/>
-      <c r="E42" s="28"/>
+      <c r="E42" s="27"/>
       <c r="F42" s="18"/>
       <c r="J42" s="18"/>
       <c r="O42" s="14"/>
-      <c r="R42" s="26"/>
+      <c r="R42" s="25"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
@@ -2548,7 +2500,7 @@
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
-      <c r="E43" s="29"/>
+      <c r="E43" s="28"/>
       <c r="F43" s="22"/>
       <c r="G43" s="5"/>
       <c r="H43" s="14"/>
@@ -2569,7 +2521,7 @@
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
-      <c r="E44" s="27"/>
+      <c r="E44" s="26"/>
       <c r="F44" s="21"/>
       <c r="G44" s="5"/>
       <c r="H44" s="14"/>
@@ -2592,11 +2544,11 @@
         <v>60</v>
       </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="28"/>
+      <c r="E45" s="27"/>
       <c r="F45" s="18"/>
       <c r="J45" s="18"/>
       <c r="O45" s="14"/>
-      <c r="R45" s="26"/>
+      <c r="R45" s="25"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B46" s="12" t="s">
@@ -2604,7 +2556,7 @@
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="29"/>
+      <c r="E46" s="28"/>
       <c r="F46" s="22"/>
       <c r="G46" s="5"/>
       <c r="H46" s="14"/>
@@ -2625,7 +2577,7 @@
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="27"/>
+      <c r="E47" s="26"/>
       <c r="F47" s="21"/>
       <c r="G47" s="5"/>
       <c r="H47" s="14"/>
@@ -2645,11 +2597,11 @@
         <v>63</v>
       </c>
       <c r="D48" s="2"/>
-      <c r="E48" s="28"/>
+      <c r="E48" s="27"/>
       <c r="F48" s="18"/>
       <c r="J48" s="18"/>
       <c r="O48" s="14"/>
-      <c r="R48" s="26"/>
+      <c r="R48" s="25"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B49" s="12" t="s">
@@ -2657,7 +2609,7 @@
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
-      <c r="E49" s="29"/>
+      <c r="E49" s="28"/>
       <c r="F49" s="22"/>
       <c r="G49" s="5"/>
       <c r="H49" s="14"/>
@@ -2678,7 +2630,7 @@
       </c>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
-      <c r="E50" s="27"/>
+      <c r="E50" s="26"/>
       <c r="F50" s="21"/>
       <c r="G50" s="5"/>
       <c r="H50" s="14"/>
@@ -2701,11 +2653,11 @@
         <v>67</v>
       </c>
       <c r="D51" s="2"/>
-      <c r="E51" s="28"/>
+      <c r="E51" s="27"/>
       <c r="F51" s="18"/>
       <c r="J51" s="18"/>
       <c r="O51" s="14"/>
-      <c r="R51" s="26"/>
+      <c r="R51" s="25"/>
     </row>
     <row r="52" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B52" s="12" t="s">
@@ -2713,7 +2665,7 @@
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
-      <c r="E52" s="29"/>
+      <c r="E52" s="28"/>
       <c r="F52" s="22"/>
       <c r="G52" s="5"/>
       <c r="H52" s="14"/>
@@ -2733,11 +2685,11 @@
         <v>69</v>
       </c>
       <c r="D53" s="2"/>
-      <c r="E53" s="28"/>
+      <c r="E53" s="27"/>
       <c r="F53" s="18"/>
       <c r="J53" s="18"/>
       <c r="O53" s="14"/>
-      <c r="R53" s="26"/>
+      <c r="R53" s="25"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
@@ -2748,7 +2700,7 @@
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="29"/>
+      <c r="E54" s="28"/>
       <c r="F54" s="22"/>
       <c r="G54" s="5"/>
       <c r="H54" s="14"/>
@@ -2769,7 +2721,7 @@
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="27"/>
+      <c r="E55" s="26"/>
       <c r="F55" s="21"/>
       <c r="G55" s="5"/>
       <c r="H55" s="14"/>
@@ -2789,11 +2741,11 @@
         <v>73</v>
       </c>
       <c r="D56" s="2"/>
-      <c r="E56" s="28"/>
+      <c r="E56" s="27"/>
       <c r="F56" s="18"/>
       <c r="J56" s="18"/>
       <c r="O56" s="14"/>
-      <c r="R56" s="26"/>
+      <c r="R56" s="25"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B57" s="12" t="s">
@@ -2801,7 +2753,7 @@
       </c>
       <c r="C57" s="5"/>
       <c r="D57" s="5"/>
-      <c r="E57" s="29"/>
+      <c r="E57" s="28"/>
       <c r="F57" s="22"/>
       <c r="G57" s="5"/>
       <c r="H57" s="14"/>
@@ -2822,7 +2774,7 @@
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5"/>
-      <c r="E58" s="27"/>
+      <c r="E58" s="26"/>
       <c r="F58" s="21"/>
       <c r="G58" s="5"/>
       <c r="H58" s="14"/>
@@ -2842,11 +2794,11 @@
         <v>76</v>
       </c>
       <c r="D59" s="2"/>
-      <c r="E59" s="28"/>
+      <c r="E59" s="27"/>
       <c r="F59" s="18"/>
       <c r="J59" s="18"/>
       <c r="O59" s="14"/>
-      <c r="R59" s="26"/>
+      <c r="R59" s="25"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B60" s="12" t="s">
@@ -2854,7 +2806,7 @@
       </c>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="29"/>
+      <c r="E60" s="28"/>
       <c r="F60" s="22"/>
       <c r="G60" s="5"/>
       <c r="H60" s="14"/>
@@ -2875,7 +2827,7 @@
       </c>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="27"/>
+      <c r="E61" s="26"/>
       <c r="F61" s="21"/>
       <c r="G61" s="5"/>
       <c r="H61" s="14"/>
@@ -2895,11 +2847,11 @@
         <v>79</v>
       </c>
       <c r="D62" s="2"/>
-      <c r="E62" s="28"/>
+      <c r="E62" s="27"/>
       <c r="F62" s="18"/>
       <c r="J62" s="18"/>
       <c r="O62" s="14"/>
-      <c r="R62" s="26"/>
+      <c r="R62" s="25"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
@@ -2910,7 +2862,7 @@
       </c>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
-      <c r="E63" s="29"/>
+      <c r="E63" s="28"/>
       <c r="F63" s="22"/>
       <c r="G63" s="5"/>
       <c r="H63" s="14"/>
@@ -2933,11 +2885,11 @@
         <v>83</v>
       </c>
       <c r="D64" s="2"/>
-      <c r="E64" s="28"/>
+      <c r="E64" s="27"/>
       <c r="F64" s="18"/>
       <c r="J64" s="18"/>
       <c r="O64" s="14"/>
-      <c r="R64" s="26"/>
+      <c r="R64" s="25"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B65" s="12" t="s">
@@ -2945,7 +2897,7 @@
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
-      <c r="E65" s="29"/>
+      <c r="E65" s="28"/>
       <c r="F65" s="22"/>
       <c r="G65" s="5"/>
       <c r="H65" s="14"/>
@@ -2966,7 +2918,7 @@
       </c>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
-      <c r="E66" s="27"/>
+      <c r="E66" s="26"/>
       <c r="F66" s="21"/>
       <c r="G66" s="5"/>
       <c r="H66" s="14"/>
@@ -2986,11 +2938,11 @@
         <v>86</v>
       </c>
       <c r="D67" s="2"/>
-      <c r="E67" s="28"/>
+      <c r="E67" s="27"/>
       <c r="F67" s="18"/>
       <c r="J67" s="18"/>
       <c r="O67" s="14"/>
-      <c r="R67" s="26"/>
+      <c r="R67" s="25"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
@@ -3001,7 +2953,7 @@
       </c>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="29"/>
+      <c r="E68" s="28"/>
       <c r="F68" s="22"/>
       <c r="G68" s="5"/>
       <c r="H68" s="14"/>
@@ -3022,7 +2974,7 @@
       </c>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="27"/>
+      <c r="E69" s="26"/>
       <c r="F69" s="21"/>
       <c r="G69" s="5"/>
       <c r="H69" s="14"/>
@@ -3042,11 +2994,11 @@
         <v>90</v>
       </c>
       <c r="D70" s="2"/>
-      <c r="E70" s="28"/>
+      <c r="E70" s="27"/>
       <c r="F70" s="18"/>
       <c r="J70" s="18"/>
       <c r="O70" s="14"/>
-      <c r="R70" s="26"/>
+      <c r="R70" s="25"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
@@ -3057,7 +3009,7 @@
       </c>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
-      <c r="E71" s="29"/>
+      <c r="E71" s="28"/>
       <c r="F71" s="22"/>
       <c r="G71" s="5"/>
       <c r="H71" s="14"/>
@@ -3078,7 +3030,7 @@
       </c>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="27"/>
+      <c r="E72" s="26"/>
       <c r="F72" s="21"/>
       <c r="G72" s="5"/>
       <c r="H72" s="14"/>
@@ -3098,11 +3050,11 @@
         <v>94</v>
       </c>
       <c r="D73" s="2"/>
-      <c r="E73" s="28"/>
+      <c r="E73" s="27"/>
       <c r="F73" s="18"/>
       <c r="J73" s="18"/>
       <c r="O73" s="14"/>
-      <c r="R73" s="26"/>
+      <c r="R73" s="25"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
@@ -3110,7 +3062,7 @@
       </c>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
-      <c r="E74" s="29"/>
+      <c r="E74" s="28"/>
       <c r="F74" s="22"/>
       <c r="G74" s="5"/>
       <c r="H74" s="14"/>
@@ -3130,11 +3082,11 @@
         <v>96</v>
       </c>
       <c r="D75" s="2"/>
-      <c r="E75" s="28"/>
+      <c r="E75" s="27"/>
       <c r="F75" s="18"/>
       <c r="J75" s="18"/>
       <c r="O75" s="14"/>
-      <c r="R75" s="26"/>
+      <c r="R75" s="25"/>
     </row>
     <row r="76" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B76" s="9" t="s">
@@ -3142,7 +3094,7 @@
       </c>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
-      <c r="E76" s="29"/>
+      <c r="E76" s="28"/>
       <c r="F76" s="22"/>
       <c r="G76" s="5"/>
       <c r="H76" s="14"/>
@@ -3163,7 +3115,7 @@
       </c>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
-      <c r="E77" s="27"/>
+      <c r="E77" s="26"/>
       <c r="F77" s="21"/>
       <c r="G77" s="5"/>
       <c r="H77" s="14"/>
@@ -3186,11 +3138,11 @@
         <v>100</v>
       </c>
       <c r="D78" s="2"/>
-      <c r="E78" s="28"/>
+      <c r="E78" s="27"/>
       <c r="F78" s="18"/>
       <c r="J78" s="18"/>
       <c r="O78" s="14"/>
-      <c r="R78" s="26"/>
+      <c r="R78" s="25"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B79" s="9" t="s">
@@ -3198,7 +3150,7 @@
       </c>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
-      <c r="E79" s="29"/>
+      <c r="E79" s="28"/>
       <c r="F79" s="22"/>
       <c r="G79" s="5"/>
       <c r="H79" s="14"/>
@@ -3218,11 +3170,11 @@
         <v>102</v>
       </c>
       <c r="D80" s="2"/>
-      <c r="E80" s="28"/>
+      <c r="E80" s="27"/>
       <c r="F80" s="18"/>
       <c r="J80" s="18"/>
       <c r="O80" s="14"/>
-      <c r="R80" s="26"/>
+      <c r="R80" s="25"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B81" s="9" t="s">
@@ -3230,7 +3182,7 @@
       </c>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
-      <c r="E81" s="29"/>
+      <c r="E81" s="28"/>
       <c r="F81" s="22"/>
       <c r="G81" s="5"/>
       <c r="H81" s="14"/>
@@ -3251,7 +3203,7 @@
       </c>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
-      <c r="E82" s="27"/>
+      <c r="E82" s="26"/>
       <c r="F82" s="21"/>
       <c r="G82" s="5"/>
       <c r="H82" s="14"/>
@@ -3271,11 +3223,11 @@
         <v>105</v>
       </c>
       <c r="D83" s="2"/>
-      <c r="E83" s="28"/>
+      <c r="E83" s="27"/>
       <c r="F83" s="18"/>
       <c r="J83" s="18"/>
       <c r="O83" s="14"/>
-      <c r="R83" s="26"/>
+      <c r="R83" s="25"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B84" s="9" t="s">
@@ -3283,7 +3235,7 @@
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
-      <c r="E84" s="29"/>
+      <c r="E84" s="28"/>
       <c r="F84" s="22"/>
       <c r="G84" s="5"/>
       <c r="H84" s="14"/>
@@ -3304,7 +3256,7 @@
       </c>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
-      <c r="E85" s="27"/>
+      <c r="E85" s="26"/>
       <c r="F85" s="21"/>
       <c r="G85" s="5"/>
       <c r="H85" s="14"/>
@@ -3324,11 +3276,11 @@
         <v>108</v>
       </c>
       <c r="D86" s="2"/>
-      <c r="E86" s="28"/>
+      <c r="E86" s="27"/>
       <c r="F86" s="18"/>
       <c r="J86" s="18"/>
       <c r="O86" s="14"/>
-      <c r="R86" s="26"/>
+      <c r="R86" s="25"/>
     </row>
     <row r="87" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="9" t="s">
@@ -3336,7 +3288,7 @@
       </c>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
-      <c r="E87" s="29"/>
+      <c r="E87" s="28"/>
       <c r="F87" s="22"/>
       <c r="G87" s="5"/>
       <c r="H87" s="14"/>
@@ -3357,7 +3309,7 @@
       </c>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
-      <c r="E88" s="27"/>
+      <c r="E88" s="26"/>
       <c r="F88" s="21"/>
       <c r="G88" s="5"/>
       <c r="H88" s="14"/>
@@ -3377,11 +3329,11 @@
         <v>111</v>
       </c>
       <c r="D89" s="2"/>
-      <c r="E89" s="28"/>
+      <c r="E89" s="27"/>
       <c r="F89" s="18"/>
       <c r="J89" s="18"/>
       <c r="O89" s="14"/>
-      <c r="R89" s="26"/>
+      <c r="R89" s="25"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B90" s="9" t="s">
@@ -3389,7 +3341,7 @@
       </c>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
-      <c r="E90" s="29"/>
+      <c r="E90" s="28"/>
       <c r="F90" s="22"/>
       <c r="G90" s="5"/>
       <c r="H90" s="14"/>
@@ -3409,11 +3361,11 @@
         <v>113</v>
       </c>
       <c r="D91" s="2"/>
-      <c r="E91" s="28"/>
+      <c r="E91" s="27"/>
       <c r="F91" s="18"/>
       <c r="J91" s="18"/>
       <c r="O91" s="14"/>
-      <c r="R91" s="26"/>
+      <c r="R91" s="25"/>
     </row>
     <row r="92" spans="1:18" ht="30" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
@@ -3421,7 +3373,7 @@
       </c>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
-      <c r="E92" s="29"/>
+      <c r="E92" s="28"/>
       <c r="F92" s="22"/>
       <c r="G92" s="5"/>
       <c r="H92" s="14"/>
@@ -3445,7 +3397,7 @@
       </c>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
-      <c r="E93" s="27"/>
+      <c r="E93" s="26"/>
       <c r="F93" s="21"/>
       <c r="G93" s="5"/>
       <c r="H93" s="14"/>
@@ -3465,11 +3417,11 @@
         <v>117</v>
       </c>
       <c r="D94" s="2"/>
-      <c r="E94" s="28"/>
+      <c r="E94" s="27"/>
       <c r="F94" s="18"/>
       <c r="J94" s="18"/>
       <c r="O94" s="14"/>
-      <c r="R94" s="26"/>
+      <c r="R94" s="25"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B95" s="9" t="s">
@@ -3477,7 +3429,7 @@
       </c>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
-      <c r="E95" s="29"/>
+      <c r="E95" s="28"/>
       <c r="F95" s="22"/>
       <c r="G95" s="5"/>
       <c r="H95" s="14"/>
@@ -3498,7 +3450,7 @@
       </c>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
-      <c r="E96" s="27"/>
+      <c r="E96" s="26"/>
       <c r="F96" s="21"/>
       <c r="G96" s="5"/>
       <c r="H96" s="14"/>
@@ -3518,11 +3470,11 @@
         <v>120</v>
       </c>
       <c r="D97" s="2"/>
-      <c r="E97" s="28"/>
+      <c r="E97" s="27"/>
       <c r="F97" s="18"/>
       <c r="J97" s="18"/>
       <c r="O97" s="14"/>
-      <c r="R97" s="26"/>
+      <c r="R97" s="25"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
@@ -3530,7 +3482,7 @@
       </c>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
-      <c r="E98" s="29"/>
+      <c r="E98" s="28"/>
       <c r="F98" s="22"/>
       <c r="G98" s="5"/>
       <c r="H98" s="14"/>
@@ -3551,7 +3503,7 @@
       </c>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
-      <c r="E99" s="27"/>
+      <c r="E99" s="26"/>
       <c r="F99" s="21"/>
       <c r="G99" s="5"/>
       <c r="H99" s="14"/>
@@ -3571,11 +3523,11 @@
         <v>123</v>
       </c>
       <c r="D100" s="2"/>
-      <c r="E100" s="28"/>
+      <c r="E100" s="27"/>
       <c r="F100" s="18"/>
       <c r="J100" s="18"/>
       <c r="O100" s="14"/>
-      <c r="R100" s="26"/>
+      <c r="R100" s="25"/>
     </row>
     <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
@@ -3583,7 +3535,7 @@
       </c>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
-      <c r="E101" s="29"/>
+      <c r="E101" s="28"/>
       <c r="F101" s="22"/>
       <c r="G101" s="5"/>
       <c r="H101" s="14"/>
@@ -3606,11 +3558,11 @@
         <v>126</v>
       </c>
       <c r="D102" s="2"/>
-      <c r="E102" s="28"/>
+      <c r="E102" s="27"/>
       <c r="F102" s="18"/>
       <c r="J102" s="18"/>
       <c r="O102" s="14"/>
-      <c r="R102" s="26"/>
+      <c r="R102" s="25"/>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B103" s="9" t="s">
@@ -3618,7 +3570,7 @@
       </c>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
-      <c r="E103" s="29"/>
+      <c r="E103" s="28"/>
       <c r="F103" s="22"/>
       <c r="G103" s="5"/>
       <c r="H103" s="14"/>
@@ -3642,7 +3594,7 @@
       </c>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
-      <c r="E104" s="27"/>
+      <c r="E104" s="26"/>
       <c r="F104" s="21"/>
       <c r="G104" s="5"/>
       <c r="H104" s="14"/>
@@ -3665,11 +3617,11 @@
         <v>131</v>
       </c>
       <c r="D105" s="2"/>
-      <c r="E105" s="28"/>
+      <c r="E105" s="27"/>
       <c r="F105" s="18"/>
       <c r="J105" s="18"/>
       <c r="O105" s="14"/>
-      <c r="R105" s="26"/>
+      <c r="R105" s="25"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B106" s="9" t="s">
@@ -3677,7 +3629,7 @@
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
-      <c r="E106" s="29"/>
+      <c r="E106" s="28"/>
       <c r="F106" s="22"/>
       <c r="G106" s="5"/>
       <c r="H106" s="14"/>
@@ -3697,11 +3649,11 @@
         <v>133</v>
       </c>
       <c r="D107" s="2"/>
-      <c r="E107" s="28"/>
+      <c r="E107" s="27"/>
       <c r="F107" s="18"/>
       <c r="J107" s="18"/>
       <c r="O107" s="14"/>
-      <c r="R107" s="26"/>
+      <c r="R107" s="25"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B108" s="9" t="s">
@@ -3709,7 +3661,7 @@
       </c>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
-      <c r="E108" s="29"/>
+      <c r="E108" s="28"/>
       <c r="F108" s="22"/>
       <c r="G108" s="5"/>
       <c r="H108" s="14"/>
@@ -3730,7 +3682,7 @@
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7"/>
-      <c r="E109" s="27"/>
+      <c r="E109" s="26"/>
       <c r="F109" s="21"/>
       <c r="G109" s="7"/>
       <c r="H109" s="17"/>
@@ -3743,7 +3695,7 @@
       <c r="O109" s="14"/>
       <c r="P109" s="17"/>
       <c r="Q109" s="17"/>
-      <c r="R109" s="25"/>
+      <c r="R109" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>